<commit_message>
Fixes having a double from-path in Excel
</commit_message>
<xml_diff>
--- a/tests/data/test.xlsx
+++ b/tests/data/test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/b.janssen/Documents/wagtail-marketing-addons/tests/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/j.janssen/Sites/git-projects/wagtail-marketing-addons/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFA13B19-43A2-F449-8E33-2C58FB188AAE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4067479-D0D5-2F4E-B820-16F8FD535ECA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="260" yWindow="460" windowWidth="28240" windowHeight="16240" xr2:uid="{C0BC65F8-9BCD-C04B-8464-01D906509E45}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
   <si>
     <t>/article/10</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>/same</t>
+  </si>
+  <si>
+    <t>/resolve</t>
+  </si>
+  <si>
+    <t>/duplicate-from-path</t>
   </si>
 </sst>
 </file>
@@ -91,7 +97,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -107,7 +113,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -403,15 +409,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{083146C4-234F-D143-813A-70F599640EB0}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.5" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -464,6 +470,22 @@
         <v>6</v>
       </c>
     </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixes having a double from-path in Excel (#15)
</commit_message>
<xml_diff>
--- a/tests/data/test.xlsx
+++ b/tests/data/test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/b.janssen/Documents/wagtail-marketing-addons/tests/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/j.janssen/Sites/git-projects/wagtail-marketing-addons/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFA13B19-43A2-F449-8E33-2C58FB188AAE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4067479-D0D5-2F4E-B820-16F8FD535ECA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="260" yWindow="460" windowWidth="28240" windowHeight="16240" xr2:uid="{C0BC65F8-9BCD-C04B-8464-01D906509E45}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
   <si>
     <t>/article/10</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>/same</t>
+  </si>
+  <si>
+    <t>/resolve</t>
+  </si>
+  <si>
+    <t>/duplicate-from-path</t>
   </si>
 </sst>
 </file>
@@ -91,7 +97,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -107,7 +113,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -403,15 +409,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{083146C4-234F-D143-813A-70F599640EB0}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.5" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -464,6 +470,22 @@
         <v>6</v>
       </c>
     </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>